<commit_message>
ajout d'un  commaentaire en local
Coucou
</commit_message>
<xml_diff>
--- a/xmlToCsvFichier.xlsx
+++ b/xmlToCsvFichier.xlsx
@@ -1,13 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\JeuDeDifferences\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13545B4-B729-4B8E-968A-F0D4DBC6A2E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="xmlToCsvFichier" sheetId="1" r:id="rId3"/>
+    <sheet name="xmlToCsvFichier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6D9A3A40-123C-4C2E-9ECE-49F90F0AC080}</author>
+  </authors>
+  <commentList>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{6D9A3A40-123C-4C2E-9ECE-49F90F0AC080}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Coucou</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,65 +224,391 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="HAMIDI Ayoub" id="{FF895D47-0A96-4476-9343-507D7B976F87}" userId="HAMIDI Ayoub" providerId="None"/>
+</personList>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B10" dT="2019-05-11T08:46:16.55" personId="{FF895D47-0A96-4476-9343-507D7B976F87}" id="{6D9A3A40-123C-4C2E-9ECE-49F90F0AC080}">
+    <text>Coucou</text>
+  </threadedComment>
+</ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -339,7 +692,7 @@
       </c>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -347,7 +700,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
@@ -359,13 +712,13 @@
         <v>31</v>
       </c>
       <c r="G2" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>33</v>
@@ -374,13 +727,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N2" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>35</v>
@@ -389,7 +742,7 @@
         <v>36</v>
       </c>
       <c r="Q2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>37</v>
@@ -398,7 +751,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -406,7 +759,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>41</v>
@@ -418,13 +771,13 @@
         <v>31</v>
       </c>
       <c r="G3" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>33</v>
@@ -433,13 +786,13 @@
         <v>42</v>
       </c>
       <c r="L3" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M3" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N3" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>35</v>
@@ -448,7 +801,7 @@
         <v>36</v>
       </c>
       <c r="Q3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>37</v>
@@ -460,19 +813,19 @@
         <v>44</v>
       </c>
       <c r="U3" s="2">
-        <v>39754.0</v>
+        <v>39754</v>
       </c>
       <c r="V3" s="2">
-        <v>39769.0</v>
+        <v>39769</v>
       </c>
       <c r="W3" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -480,7 +833,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>45</v>
@@ -492,13 +845,13 @@
         <v>31</v>
       </c>
       <c r="G4" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>33</v>
@@ -507,13 +860,13 @@
         <v>42</v>
       </c>
       <c r="L4" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M4" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N4" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>35</v>
@@ -522,7 +875,7 @@
         <v>36</v>
       </c>
       <c r="Q4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>37</v>
@@ -534,19 +887,19 @@
         <v>44</v>
       </c>
       <c r="U4" s="2">
-        <v>39754.0</v>
+        <v>39754</v>
       </c>
       <c r="V4" s="2">
-        <v>39769.0</v>
+        <v>39769</v>
       </c>
       <c r="W4" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -554,7 +907,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>47</v>
@@ -566,13 +919,13 @@
         <v>31</v>
       </c>
       <c r="G5" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I5" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>33</v>
@@ -581,13 +934,13 @@
         <v>34</v>
       </c>
       <c r="L5" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M5" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N5" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>35</v>
@@ -596,7 +949,7 @@
         <v>36</v>
       </c>
       <c r="Q5" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>37</v>
@@ -608,19 +961,19 @@
         <v>49</v>
       </c>
       <c r="U5" s="2">
-        <v>39754.0</v>
+        <v>39754</v>
       </c>
       <c r="V5" s="2">
-        <v>39769.0</v>
+        <v>39769</v>
       </c>
       <c r="W5" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -628,7 +981,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>47</v>
@@ -640,13 +993,13 @@
         <v>31</v>
       </c>
       <c r="G6" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I6" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>33</v>
@@ -655,13 +1008,13 @@
         <v>34</v>
       </c>
       <c r="L6" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M6" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N6" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>35</v>
@@ -670,7 +1023,7 @@
         <v>36</v>
       </c>
       <c r="Q6" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>37</v>
@@ -682,19 +1035,19 @@
         <v>50</v>
       </c>
       <c r="U6" s="2">
-        <v>39649.0</v>
+        <v>39649</v>
       </c>
       <c r="V6" s="2">
-        <v>39704.0</v>
+        <v>39704</v>
       </c>
       <c r="W6" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>37</v>
@@ -703,7 +1056,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -711,7 +1064,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>47</v>
@@ -723,13 +1076,13 @@
         <v>31</v>
       </c>
       <c r="G7" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I7" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>33</v>
@@ -738,13 +1091,13 @@
         <v>34</v>
       </c>
       <c r="L7" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M7" s="2">
-        <v>34467.0</v>
+        <v>34467</v>
       </c>
       <c r="N7" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>35</v>
@@ -753,7 +1106,7 @@
         <v>36</v>
       </c>
       <c r="Q7" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>37</v>
@@ -765,19 +1118,19 @@
         <v>50</v>
       </c>
       <c r="U7" s="2">
-        <v>39649.0</v>
+        <v>39649</v>
       </c>
       <c r="V7" s="2">
-        <v>39704.0</v>
+        <v>39704</v>
       </c>
       <c r="W7" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>37</v>
@@ -786,7 +1139,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -794,7 +1147,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>47</v>
@@ -810,7 +1163,7 @@
         <v>32</v>
       </c>
       <c r="I8" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>33</v>
@@ -819,13 +1172,13 @@
         <v>34</v>
       </c>
       <c r="L8" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M8" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N8" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>35</v>
@@ -834,7 +1187,7 @@
         <v>36</v>
       </c>
       <c r="Q8" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>37</v>
@@ -846,19 +1199,19 @@
         <v>54</v>
       </c>
       <c r="U8" s="2">
-        <v>39754.0</v>
+        <v>39754</v>
       </c>
       <c r="V8" s="2">
-        <v>39769.0</v>
+        <v>39769</v>
       </c>
       <c r="W8" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -866,7 +1219,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>47</v>
@@ -878,13 +1231,13 @@
         <v>31</v>
       </c>
       <c r="G9" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I9" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>33</v>
@@ -893,13 +1246,13 @@
         <v>34</v>
       </c>
       <c r="L9" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M9" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N9" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>35</v>
@@ -908,7 +1261,7 @@
         <v>36</v>
       </c>
       <c r="Q9" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>37</v>
@@ -920,19 +1273,19 @@
         <v>55</v>
       </c>
       <c r="U9" s="2">
-        <v>39590.0</v>
+        <v>39590</v>
       </c>
       <c r="V9" s="2">
-        <v>39977.0</v>
+        <v>39977</v>
       </c>
       <c r="W9" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y9" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="Z9" s="1" t="s">
         <v>37</v>
@@ -941,7 +1294,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -949,7 +1302,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>47</v>
@@ -961,13 +1314,13 @@
         <v>31</v>
       </c>
       <c r="G10" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I10" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>33</v>
@@ -976,13 +1329,13 @@
         <v>34</v>
       </c>
       <c r="L10" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M10" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N10" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>35</v>
@@ -991,7 +1344,7 @@
         <v>36</v>
       </c>
       <c r="Q10" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>37</v>
@@ -1003,19 +1356,19 @@
         <v>55</v>
       </c>
       <c r="U10" s="2">
-        <v>39590.0</v>
+        <v>39590</v>
       </c>
       <c r="V10" s="2">
-        <v>39977.0</v>
+        <v>39977</v>
       </c>
       <c r="W10" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y10" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="Z10" s="1" t="s">
         <v>37</v>
@@ -1024,7 +1377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1032,7 +1385,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>47</v>
@@ -1044,13 +1397,13 @@
         <v>31</v>
       </c>
       <c r="G11" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>33</v>
@@ -1059,13 +1412,13 @@
         <v>34</v>
       </c>
       <c r="L11" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M11" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N11" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>35</v>
@@ -1074,7 +1427,7 @@
         <v>36</v>
       </c>
       <c r="Q11" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>37</v>
@@ -1086,25 +1439,25 @@
         <v>49</v>
       </c>
       <c r="U11" s="2">
-        <v>39754.0</v>
+        <v>39754</v>
       </c>
       <c r="V11" s="2">
-        <v>39769.0</v>
+        <v>39769</v>
       </c>
       <c r="W11" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>47</v>
@@ -1116,13 +1469,13 @@
         <v>31</v>
       </c>
       <c r="G12" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I12" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>33</v>
@@ -1131,13 +1484,13 @@
         <v>34</v>
       </c>
       <c r="L12" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M12" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N12" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>35</v>
@@ -1146,7 +1499,7 @@
         <v>36</v>
       </c>
       <c r="Q12" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>37</v>
@@ -1158,19 +1511,19 @@
         <v>50</v>
       </c>
       <c r="U12" s="2">
-        <v>39649.0</v>
+        <v>39649</v>
       </c>
       <c r="V12" s="2">
-        <v>39704.0</v>
+        <v>39704</v>
       </c>
       <c r="W12" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y12" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>37</v>
@@ -1179,7 +1532,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -1187,7 +1540,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>47</v>
@@ -1199,13 +1552,13 @@
         <v>31</v>
       </c>
       <c r="G13" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>33</v>
@@ -1214,13 +1567,13 @@
         <v>34</v>
       </c>
       <c r="L13" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M13" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N13" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>35</v>
@@ -1229,7 +1582,7 @@
         <v>36</v>
       </c>
       <c r="Q13" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>37</v>
@@ -1241,19 +1594,19 @@
         <v>50</v>
       </c>
       <c r="U13" s="2">
-        <v>39649.0</v>
+        <v>39649</v>
       </c>
       <c r="V13" s="2">
-        <v>39704.0</v>
+        <v>39704</v>
       </c>
       <c r="W13" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y13" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>37</v>
@@ -1262,7 +1615,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1270,7 +1623,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>47</v>
@@ -1282,13 +1635,13 @@
         <v>31</v>
       </c>
       <c r="G14" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>33</v>
@@ -1297,13 +1650,13 @@
         <v>34</v>
       </c>
       <c r="L14" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M14" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N14" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>35</v>
@@ -1312,7 +1665,7 @@
         <v>36</v>
       </c>
       <c r="Q14" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>37</v>
@@ -1324,19 +1677,19 @@
         <v>54</v>
       </c>
       <c r="U14" s="2">
-        <v>39754.0</v>
+        <v>39754</v>
       </c>
       <c r="V14" s="2">
-        <v>39769.0</v>
+        <v>39769</v>
       </c>
       <c r="W14" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1344,7 +1697,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>47</v>
@@ -1356,13 +1709,13 @@
         <v>31</v>
       </c>
       <c r="G15" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>33</v>
@@ -1371,13 +1724,13 @@
         <v>34</v>
       </c>
       <c r="L15" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M15" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N15" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>35</v>
@@ -1386,7 +1739,7 @@
         <v>36</v>
       </c>
       <c r="Q15" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>37</v>
@@ -1398,19 +1751,19 @@
         <v>55</v>
       </c>
       <c r="U15" s="2">
-        <v>39590.0</v>
+        <v>39590</v>
       </c>
       <c r="V15" s="2">
-        <v>39977.0</v>
+        <v>39977</v>
       </c>
       <c r="W15" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y15" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>37</v>
@@ -1419,7 +1772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1427,7 +1780,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>47</v>
@@ -1439,13 +1792,13 @@
         <v>31</v>
       </c>
       <c r="G16" s="1">
-        <v>7.7313E7</v>
+        <v>77313000</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="1">
-        <v>35238.0</v>
+        <v>35238</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>33</v>
@@ -1454,13 +1807,13 @@
         <v>34</v>
       </c>
       <c r="L16" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="M16" s="2">
-        <v>41864.0</v>
+        <v>41864</v>
       </c>
       <c r="N16" s="2">
-        <v>41870.0</v>
+        <v>41870</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>35</v>
@@ -1469,7 +1822,7 @@
         <v>36</v>
       </c>
       <c r="Q16" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>37</v>
@@ -1481,19 +1834,19 @@
         <v>55</v>
       </c>
       <c r="U16" s="2">
-        <v>39590.0</v>
+        <v>39590</v>
       </c>
       <c r="V16" s="2">
-        <v>39977.0</v>
+        <v>39977</v>
       </c>
       <c r="W16" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="X16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y16" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>37</v>
@@ -1503,6 +1856,7 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>